<commit_message>
Fix profit calculation and barcode validation
</commit_message>
<xml_diff>
--- a/migration_template.xlsx
+++ b/migration_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/.gemini/antigravity/scratch/kasir-pro-supabase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09819AC2-C093-254A-AE1F-505E2E1CD9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BA25C4-BA5C-EC40-8DC9-1EB3215E6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1140" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <t>Tanggal (YYYY-MM-DD HH:mm)</t>
   </si>
@@ -49,6 +49,9 @@
     <t>cash</t>
   </si>
   <si>
+    <t>Cat Choize Hijau Tuna Adult - 800g</t>
+  </si>
+  <si>
     <t>Beauty premium Chicken and Salmon - 1kg</t>
   </si>
   <si>
@@ -67,39 +70,36 @@
     <t>Pasir Repack 1 kg</t>
   </si>
   <si>
-    <t>Bolt Donat tuna kuning 800 gr</t>
+    <t>Felibite Tuna Chicken Adult</t>
   </si>
   <si>
     <t>mister puss salmon - 500g</t>
   </si>
   <si>
+    <t>Bolt Curah</t>
+  </si>
+  <si>
     <t>Cat Choize Kuning Kitten Salmon - 1 kg</t>
   </si>
   <si>
     <t>Cat Choize Pink Kitten Tuna - 1 kg</t>
   </si>
   <si>
-    <t>Cat Choize Mother Kitten</t>
-  </si>
-  <si>
     <t>Cat Choize Oren Salmon Adult - 800 gr</t>
   </si>
   <si>
-    <t>Lezato kitten tuna- 800g</t>
-  </si>
-  <si>
     <t>excel tuna hijau</t>
   </si>
   <si>
     <t>Felibite Mom Kid Donat - 500g</t>
   </si>
   <si>
-    <t>Pasir Top 10 L</t>
-  </si>
-  <si>
     <t>Bolt Mother &amp; Kitten Salmon- 500g</t>
   </si>
   <si>
+    <t>Snack Curah kucing stik all varian rasa</t>
+  </si>
+  <si>
     <t>mister puss tuna - 500g</t>
   </si>
   <si>
@@ -115,10 +115,7 @@
     <t>Meo kaleng kitten tuna 400gr</t>
   </si>
   <si>
-    <t>lezato tuna adult 1 kg</t>
-  </si>
-  <si>
-    <t>Meo Pouch Tuna Kitten</t>
+    <t>susu kitten growsy</t>
   </si>
   <si>
     <t>Whiskas Pouch Junior Tuna Flavour</t>
@@ -130,7 +127,16 @@
     <t>Furlove Tuna Adult - 1kg</t>
   </si>
   <si>
-    <t>Furlove kitten salmon - 1kg</t>
+    <t>Life cat Kaleng tuna adult hijau 400 gr</t>
+  </si>
+  <si>
+    <t>Markotop Mom Kid Salmon Chicken</t>
+  </si>
+  <si>
+    <t>Furlove Tuna Kitten - 1kg</t>
+  </si>
+  <si>
+    <t>Markotop Mom Kid Salmon Tuna</t>
   </si>
   <si>
     <t>Life cat kaleng Tuna Kitten Pink - 400gr</t>
@@ -139,16 +145,13 @@
     <t>Life Cat Kaleng Salmon Kitten Kuning 400 gr</t>
   </si>
   <si>
-    <t>Beauty Gold Premium - 750</t>
-  </si>
-  <si>
     <t>Remov spray kutu kucing</t>
   </si>
   <si>
-    <t>Popopet shampo Cat n Dog</t>
-  </si>
-  <si>
-    <t>Bolt Dog - 1kg</t>
+    <t>Ham Meal Hamster 100gr</t>
+  </si>
+  <si>
+    <t>Meo pouch Otak² / Pempek</t>
   </si>
   <si>
     <t>Remove Parfume &amp; pelebat bulu</t>
@@ -157,25 +160,46 @@
     <t>crystal kitty tuna chicken - mother kitten</t>
   </si>
   <si>
-    <t>Meo persia kitten - 1,1 kg</t>
-  </si>
-  <si>
-    <t>maxi 500gram</t>
-  </si>
-  <si>
-    <t>Sekop pasir nude</t>
-  </si>
-  <si>
     <t>Pasir top 25L</t>
   </si>
   <si>
     <t>life cat dry - 1kg</t>
   </si>
   <si>
-    <t>meo pouch tuna Adult</t>
-  </si>
-  <si>
-    <t>Chester</t>
+    <t>Life cat kaleng chicken salmon biru - 400gr</t>
+  </si>
+  <si>
+    <t>whiskas pouch tuna-80 gr</t>
+  </si>
+  <si>
+    <t>Fish oil paket hemat</t>
+  </si>
+  <si>
+    <t>kandang ukuran 60 x 40</t>
+  </si>
+  <si>
+    <t>Kandang Besar</t>
+  </si>
+  <si>
+    <t>Oricat Kitten Tuna</t>
+  </si>
+  <si>
+    <t>Meo persian adult anti hairball - 1,1 kg</t>
+  </si>
+  <si>
+    <t>Obat cacing oxantel</t>
+  </si>
+  <si>
+    <t>oricat tuna ikan adult 800g</t>
+  </si>
+  <si>
+    <t>Bio Chicken whit Tuna</t>
+  </si>
+  <si>
+    <t>Whiskas Pouch Tuna Ikan Putih-80gr</t>
+  </si>
+  <si>
+    <t>Markotop Tuna Salmon Biru - 800g</t>
   </si>
 </sst>
 </file>
@@ -556,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,10 +622,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -615,13 +639,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -629,10 +653,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -646,13 +670,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -663,13 +687,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -677,13 +701,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -691,13 +715,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -705,13 +729,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -719,10 +743,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -733,13 +757,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -747,13 +771,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -761,13 +785,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D13">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -775,13 +799,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -789,13 +813,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -803,13 +827,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -817,13 +841,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -831,13 +855,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -845,10 +869,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -859,10 +883,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -873,13 +897,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -887,10 +911,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -901,13 +925,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -915,13 +939,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -929,13 +953,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -943,13 +967,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -957,13 +981,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -971,10 +995,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D28">
         <v>4</v>
@@ -985,13 +1009,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -999,10 +1023,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1013,13 +1037,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1027,13 +1051,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1041,13 +1065,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
@@ -1055,13 +1079,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
@@ -1069,13 +1093,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
@@ -1083,10 +1107,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1097,10 +1121,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1111,13 +1135,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
@@ -1125,10 +1149,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1139,10 +1163,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1153,13 +1177,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
         <v>8</v>
@@ -1167,10 +1191,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C42" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1181,34 +1205,146 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>46041.4375</v>
+        <v>46044.4375</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>46044.4375</v>
+      </c>
+      <c r="C52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: implement staff onboarding edge function
</commit_message>
<xml_diff>
--- a/migration_template.xlsx
+++ b/migration_template.xlsx
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/.gemini/antigravity/scratch/kasir-pro-supabase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BA25C4-BA5C-EC40-8DC9-1EB3215E6474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA252291-2519-DA49-A1CF-AA18999154F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1140" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Transaksi" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>Tanggal (YYYY-MM-DD HH:mm)</t>
   </si>
@@ -70,39 +82,33 @@
     <t>Pasir Repack 1 kg</t>
   </si>
   <si>
-    <t>Felibite Tuna Chicken Adult</t>
+    <t>Bolt Donat tuna kuning 800 gr</t>
   </si>
   <si>
     <t>mister puss salmon - 500g</t>
   </si>
   <si>
-    <t>Bolt Curah</t>
-  </si>
-  <si>
     <t>Cat Choize Kuning Kitten Salmon - 1 kg</t>
   </si>
   <si>
     <t>Cat Choize Pink Kitten Tuna - 1 kg</t>
   </si>
   <si>
+    <t>Cat Choize Mother Kitten</t>
+  </si>
+  <si>
     <t>Cat Choize Oren Salmon Adult - 800 gr</t>
   </si>
   <si>
     <t>excel tuna hijau</t>
   </si>
   <si>
-    <t>Felibite Mom Kid Donat - 500g</t>
-  </si>
-  <si>
     <t>Bolt Mother &amp; Kitten Salmon- 500g</t>
   </si>
   <si>
     <t>Snack Curah kucing stik all varian rasa</t>
   </si>
   <si>
-    <t>mister puss tuna - 500g</t>
-  </si>
-  <si>
     <t>Maxi 1kg</t>
   </si>
   <si>
@@ -112,94 +118,76 @@
     <t>Pasir Top 5 L</t>
   </si>
   <si>
-    <t>Meo kaleng kitten tuna 400gr</t>
+    <t>Felibite Mom Kid Ikan</t>
   </si>
   <si>
     <t>susu kitten growsy</t>
   </si>
   <si>
+    <t>Meo Pouch Tuna Kitten</t>
+  </si>
+  <si>
     <t>Whiskas Pouch Junior Tuna Flavour</t>
   </si>
   <si>
     <t>Nice Tuna Adult 800 gr</t>
   </si>
   <si>
-    <t>Furlove Tuna Adult - 1kg</t>
-  </si>
-  <si>
     <t>Life cat Kaleng tuna adult hijau 400 gr</t>
   </si>
   <si>
-    <t>Markotop Mom Kid Salmon Chicken</t>
+    <t>Furlove kitten salmon - 1kg</t>
   </si>
   <si>
     <t>Furlove Tuna Kitten - 1kg</t>
   </si>
   <si>
-    <t>Markotop Mom Kid Salmon Tuna</t>
-  </si>
-  <si>
     <t>Life cat kaleng Tuna Kitten Pink - 400gr</t>
   </si>
   <si>
-    <t>Life Cat Kaleng Salmon Kitten Kuning 400 gr</t>
-  </si>
-  <si>
-    <t>Remov spray kutu kucing</t>
-  </si>
-  <si>
-    <t>Ham Meal Hamster 100gr</t>
+    <t>Susu Top Growth</t>
+  </si>
+  <si>
+    <t>lezato salmon adult</t>
   </si>
   <si>
     <t>Meo pouch Otak² / Pempek</t>
   </si>
   <si>
-    <t>Remove Parfume &amp; pelebat bulu</t>
-  </si>
-  <si>
     <t>crystal kitty tuna chicken - mother kitten</t>
   </si>
   <si>
-    <t>Pasir top 25L</t>
-  </si>
-  <si>
-    <t>life cat dry - 1kg</t>
-  </si>
-  <si>
-    <t>Life cat kaleng chicken salmon biru - 400gr</t>
+    <t>Chester</t>
+  </si>
+  <si>
+    <t>Excel Salmon Kuning</t>
+  </si>
+  <si>
+    <t>Pasir Taro 10 liter</t>
   </si>
   <si>
     <t>whiskas pouch tuna-80 gr</t>
   </si>
   <si>
-    <t>Fish oil paket hemat</t>
-  </si>
-  <si>
-    <t>kandang ukuran 60 x 40</t>
-  </si>
-  <si>
-    <t>Kandang Besar</t>
-  </si>
-  <si>
-    <t>Oricat Kitten Tuna</t>
-  </si>
-  <si>
-    <t>Meo persian adult anti hairball - 1,1 kg</t>
-  </si>
-  <si>
-    <t>Obat cacing oxantel</t>
-  </si>
-  <si>
-    <t>oricat tuna ikan adult 800g</t>
-  </si>
-  <si>
-    <t>Bio Chicken whit Tuna</t>
-  </si>
-  <si>
-    <t>Whiskas Pouch Tuna Ikan Putih-80gr</t>
-  </si>
-  <si>
-    <t>Markotop Tuna Salmon Biru - 800g</t>
+    <t>Bio Salmon</t>
+  </si>
+  <si>
+    <t>Disposable syringe 3 cc/mL</t>
+  </si>
+  <si>
+    <t>Pasir Junior 5 L</t>
+  </si>
+  <si>
+    <t>Captain Cat Salmon Chicken</t>
+  </si>
+  <si>
+    <t>Bio Chicken with Scallops</t>
+  </si>
+  <si>
+    <t>crystal kitty adult</t>
+  </si>
+  <si>
+    <t>Markotop pouch Tuna Salmon</t>
   </si>
 </sst>
 </file>
@@ -209,13 +197,19 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -238,9 +232,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,13 +617,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
+        <v>46053.4375</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -639,13 +634,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -653,13 +648,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -670,13 +665,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -687,13 +682,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -701,13 +696,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -715,10 +710,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -729,13 +724,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -743,13 +738,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -757,13 +752,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -771,13 +766,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -785,10 +780,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -799,13 +794,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -813,13 +808,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -827,13 +822,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -841,10 +836,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -855,13 +850,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -869,13 +864,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -883,13 +878,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -897,13 +892,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -911,10 +906,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -925,13 +920,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -939,13 +934,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -953,13 +948,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -967,13 +962,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -981,7 +976,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -995,13 +990,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -1009,13 +1004,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -1023,10 +1018,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1037,13 +1032,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1051,13 +1046,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1065,13 +1060,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
@@ -1079,10 +1074,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1093,7 +1088,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C35" t="s">
         <v>45</v>
@@ -1107,10 +1102,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1121,10 +1116,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1135,10 +1130,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1149,13 +1144,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
@@ -1163,13 +1158,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F40" t="s">
         <v>8</v>
@@ -1177,10 +1172,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1191,13 +1186,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
@@ -1205,13 +1200,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F43" t="s">
         <v>8</v>
@@ -1219,10 +1214,10 @@
     </row>
     <row r="44" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>46044.4375</v>
+        <v>46053.4375</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1232,119 +1227,58 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>8</v>
-      </c>
+      <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>8</v>
-      </c>
+      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C47" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>8</v>
-      </c>
+      <c r="A47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C48" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="F50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C51" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51">
-        <v>2</v>
-      </c>
-      <c r="F51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>46044.4375</v>
-      </c>
-      <c r="C52" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add manual refresh button to POS header and mobile view
</commit_message>
<xml_diff>
--- a/migration_template.xlsx
+++ b/migration_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/.gemini/antigravity/scratch/kasir-pro-supabase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA252291-2519-DA49-A1CF-AA18999154F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006FF3B2-F1C5-E948-8133-E7183517D2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1140" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t>Tanggal (YYYY-MM-DD HH:mm)</t>
   </si>
@@ -82,12 +82,18 @@
     <t>Pasir Repack 1 kg</t>
   </si>
   <si>
+    <t>Felibite Tuna Chicken Adult</t>
+  </si>
+  <si>
     <t>Bolt Donat tuna kuning 800 gr</t>
   </si>
   <si>
     <t>mister puss salmon - 500g</t>
   </si>
   <si>
+    <t>Bolt Curah</t>
+  </si>
+  <si>
     <t>Cat Choize Kuning Kitten Salmon - 1 kg</t>
   </si>
   <si>
@@ -103,24 +109,45 @@
     <t>excel tuna hijau</t>
   </si>
   <si>
+    <t>kalung hitam</t>
+  </si>
+  <si>
+    <t>Markotop pouch Tuna</t>
+  </si>
+  <si>
+    <t>Pasir Top 10 L</t>
+  </si>
+  <si>
     <t>Bolt Mother &amp; Kitten Salmon- 500g</t>
   </si>
   <si>
     <t>Snack Curah kucing stik all varian rasa</t>
   </si>
   <si>
+    <t>mister puss tuna - 500g</t>
+  </si>
+  <si>
     <t>Maxi 1kg</t>
   </si>
   <si>
     <t>excel tuna ungu</t>
   </si>
   <si>
-    <t>Pasir Top 5 L</t>
+    <t>Underpad 60 x 60 - L</t>
   </si>
   <si>
     <t>Felibite Mom Kid Ikan</t>
   </si>
   <si>
+    <t>kalung ungu</t>
+  </si>
+  <si>
+    <t>lezato tuna adult 1 kg</t>
+  </si>
+  <si>
+    <t>Whiskas Kaleng Tuna-400gr</t>
+  </si>
+  <si>
     <t>susu kitten growsy</t>
   </si>
   <si>
@@ -133,61 +160,67 @@
     <t>Nice Tuna Adult 800 gr</t>
   </si>
   <si>
-    <t>Life cat Kaleng tuna adult hijau 400 gr</t>
-  </si>
-  <si>
-    <t>Furlove kitten salmon - 1kg</t>
-  </si>
-  <si>
-    <t>Furlove Tuna Kitten - 1kg</t>
-  </si>
-  <si>
-    <t>Life cat kaleng Tuna Kitten Pink - 400gr</t>
+    <t>Markotop Mom Kid Salmon Chicken</t>
+  </si>
+  <si>
+    <t>Markotop Mom Kid Salmon Tuna</t>
   </si>
   <si>
     <t>Susu Top Growth</t>
   </si>
   <si>
+    <t>Remov spray kutu kucing</t>
+  </si>
+  <si>
     <t>lezato salmon adult</t>
   </si>
   <si>
-    <t>Meo pouch Otak² / Pempek</t>
+    <t>Bolt Dog - 1kg</t>
   </si>
   <si>
     <t>crystal kitty tuna chicken - mother kitten</t>
   </si>
   <si>
+    <t>maxi 500gram</t>
+  </si>
+  <si>
+    <t>Pasir top 25L</t>
+  </si>
+  <si>
+    <t>life cat dry - 1kg</t>
+  </si>
+  <si>
     <t>Chester</t>
   </si>
   <si>
-    <t>Excel Salmon Kuning</t>
-  </si>
-  <si>
-    <t>Pasir Taro 10 liter</t>
-  </si>
-  <si>
     <t>whiskas pouch tuna-80 gr</t>
   </si>
   <si>
-    <t>Bio Salmon</t>
-  </si>
-  <si>
-    <t>Disposable syringe 3 cc/mL</t>
-  </si>
-  <si>
-    <t>Pasir Junior 5 L</t>
-  </si>
-  <si>
-    <t>Captain Cat Salmon Chicken</t>
-  </si>
-  <si>
-    <t>Bio Chicken with Scallops</t>
-  </si>
-  <si>
-    <t>crystal kitty adult</t>
-  </si>
-  <si>
-    <t>Markotop pouch Tuna Salmon</t>
+    <t>Obat Diare Royal Care</t>
+  </si>
+  <si>
+    <t>Fish oil paket hemat</t>
+  </si>
+  <si>
+    <t>Meo persian adult anti hairball - 1,1 kg</t>
+  </si>
+  <si>
+    <t>Pasir Taro 5 L</t>
+  </si>
+  <si>
+    <t>Pet Shampoo</t>
+  </si>
+  <si>
+    <t>dot kucing</t>
+  </si>
+  <si>
+    <t>Markotop pouch MK Tuna Chicken</t>
+  </si>
+  <si>
+    <t>Baju green/purple princess M</t>
+  </si>
+  <si>
+    <t>Pasir Junior 25 L</t>
   </si>
 </sst>
 </file>
@@ -195,21 +228,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -232,10 +259,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39:F44"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,13 +643,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>46053.4375</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>46054.4375</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -634,10 +660,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -648,10 +674,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -665,13 +691,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -682,13 +708,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -696,13 +722,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -710,13 +736,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -724,13 +750,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -738,13 +764,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -752,13 +778,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -766,13 +792,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -780,13 +806,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -794,10 +820,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -808,10 +834,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -822,13 +848,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -836,13 +862,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -850,13 +876,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -864,13 +890,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -878,13 +904,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -892,13 +918,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -906,10 +932,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -920,13 +946,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -934,13 +960,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -948,13 +974,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -962,10 +988,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -976,13 +1002,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -990,10 +1016,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1004,13 +1030,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -1018,13 +1044,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
@@ -1032,13 +1058,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1046,13 +1072,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1060,13 +1086,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
@@ -1074,13 +1100,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
@@ -1088,13 +1114,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
@@ -1102,13 +1128,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
@@ -1116,10 +1142,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1130,13 +1156,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C38" t="s">
         <v>39</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
@@ -1144,13 +1170,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C39" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
@@ -1158,13 +1184,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="s">
         <v>8</v>
@@ -1172,13 +1198,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F41" t="s">
         <v>8</v>
@@ -1186,13 +1212,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
@@ -1200,13 +1226,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
         <v>8</v>
@@ -1214,71 +1240,189 @@
     </row>
     <row r="44" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>46053.4375</v>
+        <v>46054.4375</v>
       </c>
       <c r="C44" t="s">
         <v>28</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C50" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>46054.4375</v>
+      </c>
+      <c r="C55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: Dashboard charts now use RPC to bypass RLS
- Created get_dashboard_monthly_summary RPC with SECURITY DEFINER
- Updated DashboardCharts.jsx to use RPC instead of direct table queries
- Fixed cash_flow type filter (out instead of expense)
- This fixes February data not showing in charts
</commit_message>
<xml_diff>
--- a/migration_template.xlsx
+++ b/migration_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/.gemini/antigravity/scratch/kasir-pro-supabase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006FF3B2-F1C5-E948-8133-E7183517D2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC497B0-3715-4F45-B36F-D99ABAEA7E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1140" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>Tanggal (YYYY-MM-DD HH:mm)</t>
   </si>
@@ -61,174 +61,73 @@
     <t>cash</t>
   </si>
   <si>
-    <t>Cat Choize Hijau Tuna Adult - 800g</t>
-  </si>
-  <si>
-    <t>Beauty premium Chicken and Salmon - 1kg</t>
-  </si>
-  <si>
-    <t>Bolt Salmon - 800g</t>
-  </si>
-  <si>
-    <t>Excel mother kitten</t>
-  </si>
-  <si>
-    <t>Bolt Tuna - 800g</t>
-  </si>
-  <si>
-    <t>Bolt Mother Kitten tuna- 500g</t>
-  </si>
-  <si>
-    <t>Pasir Repack 1 kg</t>
-  </si>
-  <si>
-    <t>Felibite Tuna Chicken Adult</t>
-  </si>
-  <si>
-    <t>Bolt Donat tuna kuning 800 gr</t>
-  </si>
-  <si>
-    <t>mister puss salmon - 500g</t>
-  </si>
-  <si>
-    <t>Bolt Curah</t>
-  </si>
-  <si>
-    <t>Cat Choize Kuning Kitten Salmon - 1 kg</t>
-  </si>
-  <si>
-    <t>Cat Choize Pink Kitten Tuna - 1 kg</t>
-  </si>
-  <si>
-    <t>Cat Choize Mother Kitten</t>
-  </si>
-  <si>
-    <t>Cat Choize Oren Salmon Adult - 800 gr</t>
-  </si>
-  <si>
-    <t>excel tuna hijau</t>
-  </si>
-  <si>
-    <t>kalung hitam</t>
-  </si>
-  <si>
-    <t>Markotop pouch Tuna</t>
-  </si>
-  <si>
-    <t>Pasir Top 10 L</t>
-  </si>
-  <si>
-    <t>Bolt Mother &amp; Kitten Salmon- 500g</t>
-  </si>
-  <si>
-    <t>Snack Curah kucing stik all varian rasa</t>
-  </si>
-  <si>
-    <t>mister puss tuna - 500g</t>
-  </si>
-  <si>
-    <t>Maxi 1kg</t>
-  </si>
-  <si>
-    <t>excel tuna ungu</t>
-  </si>
-  <si>
-    <t>Underpad 60 x 60 - L</t>
-  </si>
-  <si>
-    <t>Felibite Mom Kid Ikan</t>
-  </si>
-  <si>
-    <t>kalung ungu</t>
-  </si>
-  <si>
-    <t>lezato tuna adult 1 kg</t>
-  </si>
-  <si>
-    <t>Whiskas Kaleng Tuna-400gr</t>
-  </si>
-  <si>
-    <t>susu kitten growsy</t>
-  </si>
-  <si>
-    <t>Meo Pouch Tuna Kitten</t>
-  </si>
-  <si>
-    <t>Whiskas Pouch Junior Tuna Flavour</t>
-  </si>
-  <si>
-    <t>Nice Tuna Adult 800 gr</t>
-  </si>
-  <si>
-    <t>Markotop Mom Kid Salmon Chicken</t>
-  </si>
-  <si>
-    <t>Markotop Mom Kid Salmon Tuna</t>
-  </si>
-  <si>
-    <t>Susu Top Growth</t>
-  </si>
-  <si>
-    <t>Remov spray kutu kucing</t>
-  </si>
-  <si>
-    <t>lezato salmon adult</t>
-  </si>
-  <si>
-    <t>Bolt Dog - 1kg</t>
-  </si>
-  <si>
-    <t>crystal kitty tuna chicken - mother kitten</t>
-  </si>
-  <si>
-    <t>maxi 500gram</t>
-  </si>
-  <si>
-    <t>Pasir top 25L</t>
-  </si>
-  <si>
-    <t>life cat dry - 1kg</t>
-  </si>
-  <si>
-    <t>Chester</t>
-  </si>
-  <si>
-    <t>whiskas pouch tuna-80 gr</t>
-  </si>
-  <si>
-    <t>Obat Diare Royal Care</t>
-  </si>
-  <si>
-    <t>Fish oil paket hemat</t>
-  </si>
-  <si>
-    <t>Meo persian adult anti hairball - 1,1 kg</t>
-  </si>
-  <si>
-    <t>Pasir Taro 5 L</t>
-  </si>
-  <si>
-    <t>Pet Shampoo</t>
-  </si>
-  <si>
-    <t>dot kucing</t>
-  </si>
-  <si>
-    <t>Markotop pouch MK Tuna Chicken</t>
-  </si>
-  <si>
-    <t>Baju green/purple princess M</t>
-  </si>
-  <si>
-    <t>Pasir Junior 25 L</t>
+    <t>tmptpknpnk</t>
+  </si>
+  <si>
+    <t>1kg</t>
+  </si>
+  <si>
+    <t>haagdh</t>
+  </si>
+  <si>
+    <t>snackCurahall</t>
+  </si>
+  <si>
+    <t>psrrpk1kg</t>
+  </si>
+  <si>
+    <t>bpccs1kg</t>
+  </si>
+  <si>
+    <t>fishoilpakethemat</t>
+  </si>
+  <si>
+    <t>kuningreflektif</t>
+  </si>
+  <si>
+    <t>hitamreflektif</t>
+  </si>
+  <si>
+    <t>salepscabies</t>
+  </si>
+  <si>
+    <t>lkkhg</t>
+  </si>
+  <si>
+    <t>kd75</t>
+  </si>
+  <si>
+    <t>prlnd5l</t>
+  </si>
+  <si>
+    <t>optima5</t>
+  </si>
+  <si>
+    <t>ltrbxkcl</t>
+  </si>
+  <si>
+    <t>skppsrnd</t>
+  </si>
+  <si>
+    <t>jjaygdb</t>
+  </si>
+  <si>
+    <t>tmptpknnd</t>
+  </si>
+  <si>
+    <t>prlnd10l</t>
+  </si>
+  <si>
+    <t>gdghh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -259,9 +158,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,13 +545,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C2" s="2">
+        <v>8994109204464</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -660,13 +562,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C3" s="2">
+        <v>8994125000361</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -674,13 +576,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C4" s="2">
+        <v>8993374326994</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -691,13 +593,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8850477015524</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -708,13 +610,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8850477005129</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -722,13 +624,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8850477017160</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -736,13 +638,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8993374326970</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -750,13 +652,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -764,13 +666,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8994109204334</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -778,13 +680,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -792,13 +694,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8994109204433</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -806,13 +708,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8850477019751</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -820,13 +722,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C14" s="2">
+        <v>8994409101371</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -834,13 +736,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8994125000439</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -848,13 +750,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8997212340623</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -862,13 +764,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C17" s="2">
+        <v>8993374326116</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -876,10 +778,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C18" s="2">
+        <v>8994125000125</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -890,13 +792,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C19" s="2">
+        <v>8994125000064</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -904,13 +806,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C20" s="2">
+        <v>12345</v>
       </c>
       <c r="D20">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -918,10 +820,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C21" s="2">
+        <v>8997215690015</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -932,13 +834,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6974756720335</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
@@ -946,13 +848,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -960,10 +862,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -974,13 +876,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C25" t="s">
-        <v>49</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -988,13 +890,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C26" t="s">
-        <v>43</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1002,13 +904,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C27" t="s">
-        <v>27</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C27" s="2">
+        <v>8993374326987</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -1016,13 +918,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C28" t="s">
-        <v>37</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C28" s="2">
+        <v>8993374325690</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -1030,13 +932,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C29" t="s">
-        <v>56</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -1044,10 +946,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C30" t="s">
-        <v>54</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1058,13 +960,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C31" t="s">
-        <v>11</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C31" s="2">
+        <v>8994125000750</v>
       </c>
       <c r="D31">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1072,13 +974,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C32" s="2">
+        <v>8853301550048</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1086,10 +988,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C33" t="s">
-        <v>40</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D33">
         <v>2</v>
@@ -1100,13 +1002,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C34" t="s">
-        <v>15</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C34" s="2">
+        <v>745114272621</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
@@ -1114,13 +1016,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C35" t="s">
-        <v>44</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
@@ -1128,13 +1030,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C36" t="s">
-        <v>34</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
@@ -1142,10 +1044,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C37" t="s">
-        <v>53</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1156,10 +1058,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C38" t="s">
-        <v>39</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C38" s="2">
+        <v>745114272669</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -1170,10 +1072,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C39" t="s">
-        <v>57</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -1184,10 +1086,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C40" t="s">
-        <v>24</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C40" s="2">
+        <v>899600540029</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1198,13 +1100,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C41" t="s">
-        <v>10</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F41" t="s">
         <v>8</v>
@@ -1212,10 +1114,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C42" t="s">
-        <v>22</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1226,10 +1128,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C43" t="s">
-        <v>14</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -1240,13 +1142,13 @@
     </row>
     <row r="44" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C44" t="s">
-        <v>28</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2222</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
         <v>8</v>
@@ -1254,13 +1156,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C45" t="s">
-        <v>47</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1111</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
         <v>8</v>
@@ -1268,13 +1170,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C46" t="s">
-        <v>42</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1109202025022</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F46" t="s">
         <v>8</v>
@@ -1282,10 +1184,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C47" t="s">
-        <v>32</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1296,10 +1198,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C48" t="s">
-        <v>36</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C48" s="2">
+        <v>745114272980</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1310,10 +1212,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C49" t="s">
-        <v>61</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1324,10 +1226,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C50" t="s">
-        <v>31</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C50" s="2">
+        <v>8853301742504</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1338,10 +1240,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C51" t="s">
-        <v>52</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1352,10 +1254,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C52" t="s">
-        <v>59</v>
+        <v>46056.4375</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1365,46 +1267,13 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>8</v>
-      </c>
+      <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C54" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
-        <v>8</v>
-      </c>
+      <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>46054.4375</v>
-      </c>
-      <c r="C55" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="F55" t="s">
-        <v>8</v>
-      </c>
+      <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
@@ -1420,9 +1289,6 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement Dot Matrix support and fix ghost transactions
</commit_message>
<xml_diff>
--- a/migration_template.xlsx
+++ b/migration_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamal/.gemini/antigravity/scratch/kasir-pro-supabase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC497B0-3715-4F45-B36F-D99ABAEA7E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8977611-38B1-BA42-A307-843449E891F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1140" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
   <si>
     <t>Tanggal (YYYY-MM-DD HH:mm)</t>
   </si>
@@ -61,12 +61,6 @@
     <t>cash</t>
   </si>
   <si>
-    <t>tmptpknpnk</t>
-  </si>
-  <si>
-    <t>1kg</t>
-  </si>
-  <si>
     <t>haagdh</t>
   </si>
   <si>
@@ -79,46 +73,34 @@
     <t>bpccs1kg</t>
   </si>
   <si>
-    <t>fishoilpakethemat</t>
-  </si>
-  <si>
-    <t>kuningreflektif</t>
-  </si>
-  <si>
-    <t>hitamreflektif</t>
-  </si>
-  <si>
-    <t>salepscabies</t>
-  </si>
-  <si>
     <t>lkkhg</t>
   </si>
   <si>
-    <t>kd75</t>
-  </si>
-  <si>
     <t>prlnd5l</t>
   </si>
   <si>
     <t>optima5</t>
   </si>
   <si>
-    <t>ltrbxkcl</t>
-  </si>
-  <si>
     <t>skppsrnd</t>
   </si>
   <si>
-    <t>jjaygdb</t>
-  </si>
-  <si>
-    <t>tmptpknnd</t>
-  </si>
-  <si>
-    <t>prlnd10l</t>
-  </si>
-  <si>
     <t>gdghh</t>
+  </si>
+  <si>
+    <t>ahshff</t>
+  </si>
+  <si>
+    <t>hagytqr</t>
+  </si>
+  <si>
+    <t>pokhtr</t>
+  </si>
+  <si>
+    <t>bcpgp800gr</t>
+  </si>
+  <si>
+    <t>syrng3cc</t>
   </si>
 </sst>
 </file>
@@ -158,12 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,10 +528,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8994109204464</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C2" s="3">
+        <v>8997206610220</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -562,13 +545,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C3" s="2">
-        <v>8994125000361</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -576,13 +559,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C4" s="2">
-        <v>8993374326994</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -593,13 +576,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C5" s="2">
-        <v>8850477015524</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8993374326970</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -610,13 +593,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C6" s="2">
-        <v>8850477005129</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8879220543145</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -624,13 +607,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C7" s="2">
-        <v>8850477017160</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8994125000361</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -638,13 +621,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C8" s="2">
-        <v>8993374326970</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C8" s="3">
+        <v>8994125000439</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -652,13 +635,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C9" s="3">
+        <v>6974756720335</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -666,13 +649,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C10" s="2">
-        <v>8994109204334</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -680,13 +663,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C11" s="3">
+        <v>745114272737</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -694,13 +677,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8994109204433</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C12" s="3">
+        <v>8850477019751</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -708,13 +691,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C13" s="2">
-        <v>8850477019751</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8993374326994</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -722,10 +705,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C14" s="2">
-        <v>8994409101371</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C14" s="3">
+        <v>8994125000125</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -736,13 +719,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C15" s="2">
-        <v>8994125000439</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C15" s="3">
+        <v>745114272669</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -750,13 +733,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C16" s="2">
-        <v>8997212340623</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C16" s="3">
+        <v>8993374326987</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -764,10 +747,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C17" s="2">
-        <v>8993374326116</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C17" s="3">
+        <v>8994109204334</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -778,10 +761,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C18" s="2">
-        <v>8994125000125</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -792,13 +775,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C19" s="2">
-        <v>8994125000064</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -806,10 +789,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C20" s="2">
-        <v>12345</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -820,13 +803,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C21" s="2">
-        <v>8997215690015</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -834,10 +817,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C22" s="2">
-        <v>6974756720335</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C22" s="3">
+        <v>745114272621</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -848,10 +831,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>15</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -862,13 +845,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>16</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C24" s="3">
+        <v>8994109204433</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -876,13 +859,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>17</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C25" s="3">
+        <v>8853301550048</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -890,13 +873,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>10</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C26" s="3">
+        <v>8994409101944</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -904,13 +887,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C27" s="2">
-        <v>8993374326987</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C27" s="3">
+        <v>8879220543121</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -918,13 +901,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C28" s="2">
-        <v>8993374325690</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -932,13 +915,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>14</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C29" s="3">
+        <v>6974756720311</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -946,13 +929,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C30" s="3">
+        <v>8850477005129</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
@@ -960,13 +943,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C31" s="2">
-        <v>8994125000750</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C31" s="3">
+        <v>8997212340623</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -974,10 +957,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C32" s="2">
-        <v>8853301550048</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -988,13 +971,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C33" s="3">
+        <v>745114272638</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
@@ -1002,13 +985,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C34" s="2">
-        <v>745114272621</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C34" s="3">
+        <v>745114272720</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
@@ -1016,10 +999,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C35" s="3">
+        <v>8994409101371</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1030,13 +1013,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>9</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C36" s="3">
+        <v>8879220546894</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
@@ -1044,10 +1027,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>21</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C37" s="3">
+        <v>745114272997</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1058,13 +1041,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C38" s="2">
-        <v>745114272669</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C38" s="3">
+        <v>8994125001115</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
@@ -1072,10 +1055,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>12</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -1086,10 +1069,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C40" s="2">
-        <v>899600540029</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C40" s="3">
+        <v>8993374325690</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1100,10 +1083,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>22</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -1114,10 +1097,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>23</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1126,12 +1109,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>24</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1109202025022</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -1140,12 +1123,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C44" s="2">
-        <v>2222</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1156,10 +1139,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1111</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C45" s="3">
+        <v>8994409101548</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1170,13 +1153,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C46" s="2">
-        <v>1109202025022</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C46" s="3">
+        <v>8850477017672</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
         <v>8</v>
@@ -1184,10 +1167,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>25</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C47" s="3">
+        <v>8853301742504</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1198,10 +1181,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C48" s="2">
-        <v>745114272980</v>
+        <v>46064.4375</v>
+      </c>
+      <c r="C48" s="3">
+        <v>8994109204464</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1210,84 +1193,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C50" s="2">
-        <v>8853301742504</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="F50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>46056.4375</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
     </row>
   </sheetData>

</xml_diff>